<commit_message>
made some css changes made report changes
</commit_message>
<xml_diff>
--- a/Planning Report/Survey results.xlsx
+++ b/Planning Report/Survey results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordan\Desktop\CI301-repo\CI301\Planning Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE99F66-82FD-477B-97C9-96C859CFFD48}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750498C9-58B2-48FA-AEF7-3B5261EFCC5A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32730" yWindow="1485" windowWidth="24345" windowHeight="14040" xr2:uid="{26F6B304-45BF-4D62-AF48-1FFCEE404A08}"/>
+    <workbookView xWindow="29970" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{26F6B304-45BF-4D62-AF48-1FFCEE404A08}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4517,8 +4517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFFBE274-F03F-4904-9E53-5DBF4D1BAC51}">
   <dimension ref="A2:AE91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AH18" sqref="AH18"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O102" sqref="O102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>

</xml_diff>